<commit_message>
Alcuni piccoli aggiustamenti; rimane da sistemare la legenda in termini di veicoli ed approfondire riguardo il codice consegna 39666 (probabilmente Commerciale IS - in tal caso da gestire in maniera peculiare in quanto è presente sia in commesse a zona zero sia in commesse a zona non zero - il che complica il codice)
</commit_message>
<xml_diff>
--- a/PS-VRP/OUTPUT_TEST/insert_intra.xlsx
+++ b/PS-VRP/OUTPUT_TEST/insert_intra.xlsx
@@ -1019,41 +1019,41 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>251742</v>
+        <v>251284</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>30</v>
+        <v>40.5</v>
       </c>
       <c r="D9" t="n">
-        <v>134.8524590163935</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:00:00</t>
+          <t>2025-05-09 07:00:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-05-08 07:30:00</t>
+          <t>2025-05-09 07:40:30</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>8226</v>
+        <v>16340</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1062,17 +1062,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M9" t="n">
         <v>70</v>
       </c>
       <c r="N9" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1080,57 +1080,57 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>39749</v>
+        <v>39747</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R9" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-1.526104797974537</v>
       </c>
       <c r="S9" s="1" t="n">
-        <v>-1.406147540983796</v>
+        <v>-1.526104797974537</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>251840</v>
+        <v>251373</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>25</v>
+        <v>34.5</v>
       </c>
       <c r="D10" t="n">
-        <v>93.67213114754098</v>
+        <v>310.8</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-05-08 09:44:51</t>
+          <t>2025-05-09 12:37:35</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-09 13:12:05</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-05-08 10:09:51</t>
+          <t>2025-05-09 13:12:05</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-12 10:22:53</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>5714</v>
+        <v>17094</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1148,66 +1148,61 @@
       <c r="M10" t="n">
         <v>70</v>
       </c>
-      <c r="N10" t="n">
-        <v>39758</v>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O10" t="n">
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>39758</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R10" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>0</v>
       </c>
       <c r="S10" s="1" t="n">
-        <v>-0.4885587431712963</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>251456</v>
+        <v>251463</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>30</v>
+        <v>32.5</v>
       </c>
       <c r="D11" t="n">
-        <v>147.5245901639344</v>
+        <v>126.6727272727273</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2025-05-08 11:43:31</t>
+          <t>2025-05-12 10:22:53</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-12 10:55:23</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-05-08 12:13:31</t>
+          <t>2025-05-12 10:55:23</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-05-08 14:41:02</t>
+          <t>2025-05-12 13:02:03</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>8999</v>
+        <v>6967</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1220,21 +1215,16 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M11" t="n">
         <v>70</v>
       </c>
-      <c r="N11" t="n">
-        <v>39746</v>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O11" t="n">
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>39746</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
@@ -1242,49 +1232,49 @@
         </is>
       </c>
       <c r="R11" s="1" t="n">
-        <v>-2.611839708564815</v>
+        <v>0</v>
       </c>
       <c r="S11" s="1" t="n">
-        <v>-2.611839708564815</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>251416</v>
+        <v>251846</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>34.5</v>
       </c>
       <c r="D12" t="n">
-        <v>183.9672131147541</v>
+        <v>207.1272727272727</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-08 14:41:02</t>
+          <t>2025-05-12 13:02:03</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-09 07:06:02</t>
+          <t>2025-05-12 13:36:33</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-05-09 07:06:02</t>
+          <t>2025-05-12 13:36:33</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-05-09 10:10:00</t>
+          <t>2025-05-13 09:03:41</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>11222</v>
+        <v>11392</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1302,9 +1292,6 @@
       <c r="M12" t="n">
         <v>70</v>
       </c>
-      <c r="N12" t="n">
-        <v>39755</v>
-      </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
@@ -1313,7 +1300,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-30 00:00:00</t>
         </is>
       </c>
       <c r="R12" s="1" t="n">
@@ -1325,41 +1312,41 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>251566</v>
+        <v>251462</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="D13" t="n">
-        <v>112.9344262295082</v>
+        <v>113.2</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2025-05-09 10:10:00</t>
+          <t>2025-05-13 09:03:41</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-05-09 10:40:00</t>
+          <t>2025-05-13 09:34:11</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-05-09 10:40:00</t>
+          <t>2025-05-13 09:34:11</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-05-09 12:32:57</t>
+          <t>2025-05-13 11:27:23</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>6889</v>
+        <v>6226</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1372,7 +1359,7 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M13" t="n">
         <v>70</v>
@@ -1385,7 +1372,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>2025-05-07 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R13" s="1" t="n">
@@ -1397,41 +1384,41 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>251424</v>
+        <v>251520</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>20</v>
+        <v>40.5</v>
       </c>
       <c r="D14" t="n">
-        <v>158.3934426229508</v>
+        <v>297.0909090909091</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-05-09 12:32:57</t>
+          <t>2025-05-13 11:27:23</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-05-09 12:52:57</t>
+          <t>2025-05-13 12:07:53</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-05-09 12:52:57</t>
+          <t>2025-05-13 12:07:53</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-05-12 07:31:20</t>
+          <t>2025-05-14 09:04:58</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>9662</v>
+        <v>16340</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1440,11 +1427,11 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>CASON ;R6</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M14" t="n">
         <v>70</v>
@@ -1457,7 +1444,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-12 00:00:00</t>
         </is>
       </c>
       <c r="R14" s="1" t="n">
@@ -1469,41 +1456,41 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>244355</v>
+        <v>251259</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>CASON</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>34.5</v>
       </c>
       <c r="D15" t="n">
-        <v>70.65573770491804</v>
+        <v>90.90909090909091</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-05-12 07:31:20</t>
+          <t>2025-05-14 09:04:58</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-05-12 07:51:20</t>
+          <t>2025-05-14 09:39:28</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-05-12 07:51:20</t>
+          <t>2025-05-14 09:39:28</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-05-12 09:02:00</t>
+          <t>2025-05-14 11:10:23</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>4310</v>
+        <v>5000</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1516,7 +1503,7 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="M15" t="n">
         <v>70</v>
@@ -1529,7 +1516,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>2025-05-08 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R15" s="1" t="n">
@@ -1541,113 +1528,117 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>251505</v>
+        <v>251706</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>233.6885245901639</v>
+        <v>50.79365079365079</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-05-12 09:02:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-05-12 09:27:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-05-12 09:27:00</t>
+          <t>2025-05-12 07:00:00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-05-12 13:20:41</t>
+          <t>2025-05-12 07:50:47</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>14255</v>
+        <v>3200</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>bobina</t>
+          <t>foglio</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>T3</t>
         </is>
       </c>
       <c r="L16" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>70</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>39764 (esterno)</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>39764</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-14 00:00:00</t>
         </is>
       </c>
       <c r="R16" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>244023</v>
+        <v>251455</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D17" t="n">
-        <v>16.34426229508197</v>
+        <v>82.765625</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2025-05-12 13:20:41</t>
+          <t>2025-05-07 07:00:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-12 13:45:41</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-05-12 13:45:41</t>
+          <t>2025-05-07 07:19:00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-05-12 14:02:01</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>997</v>
+        <v>5297</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1660,66 +1651,71 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M17" t="n">
         <v>70</v>
       </c>
-      <c r="O17" t="n">
-        <v>0</v>
+      <c r="N17" t="n">
+        <v>39749</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>2024-09-30 00:00:00</t>
+          <t>2025-04-15 00:00:00</t>
         </is>
       </c>
       <c r="R17" s="1" t="n">
-        <v>0</v>
+        <v>-0.3623372395833334</v>
       </c>
       <c r="S17" s="1" t="n">
-        <v>0</v>
+        <v>-0.3623372395833334</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>251061</v>
+        <v>251391</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>393.3934426229508</v>
+        <v>91.640625</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-12 14:02:01</t>
+          <t>2025-05-07 08:41:45</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-05-12 14:22:01</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-05-12 14:22:01</t>
+          <t>2025-05-07 08:58:45</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-05-13 12:55:25</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>23997</v>
+        <v>5865</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1728,70 +1724,75 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M18" t="n">
         <v>70</v>
       </c>
-      <c r="O18" t="n">
-        <v>0</v>
+      <c r="N18" t="n">
+        <v>39749</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P18" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R18" s="1" t="n">
-        <v>0</v>
+        <v>-0.4377821180555556</v>
       </c>
       <c r="S18" s="1" t="n">
-        <v>0</v>
+        <v>-0.4377821180555556</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>251260</v>
+        <v>251395</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D19" t="n">
-        <v>153.5901639344262</v>
+        <v>35.34375</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-05-13 12:55:25</t>
+          <t>2025-05-07 10:30:24</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-05-13 13:15:25</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-05-13 13:15:25</t>
+          <t>2025-05-07 10:47:24</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-05-14 07:49:00</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>9369</v>
+        <v>2262</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1800,7 +1801,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L19" t="n">
@@ -1809,61 +1810,66 @@
       <c r="M19" t="n">
         <v>70</v>
       </c>
-      <c r="O19" t="n">
-        <v>0</v>
+      <c r="N19" t="n">
+        <v>39749</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>2025-05-22 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R19" s="1" t="n">
-        <v>0</v>
+        <v>-0.4741319444444445</v>
       </c>
       <c r="S19" s="1" t="n">
-        <v>0</v>
+        <v>-0.4741319444444445</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>251795</v>
+        <v>251371</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>307.1967213114754</v>
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-05-14 07:49:00</t>
+          <t>2025-05-07 11:22:45</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-05-14 08:09:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-05-14 08:09:00</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-05-14 13:16:12</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>18739</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1872,70 +1878,77 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L20" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M20" t="n">
         <v>70</v>
       </c>
-      <c r="O20" t="n">
-        <v>0</v>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>39666 (esterno)</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P20" t="n">
-        <v>0</v>
+        <v>39666</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>2025-06-19 00:00:00</t>
+          <t>2025-04-24 00:00:00</t>
         </is>
       </c>
       <c r="R20" s="1" t="n">
-        <v>0</v>
+        <v>-13.48732638888889</v>
       </c>
       <c r="S20" s="1" t="n">
-        <v>0</v>
+        <v>-13.48732638888889</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>251346</v>
+        <v>251396</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>R10</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D21" t="n">
-        <v>63.26229508196721</v>
+        <v>35.34375</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2025-05-14 13:16:12</t>
+          <t>2025-05-07 11:41:45</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-05-14 13:46:12</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-05-14 13:46:12</t>
+          <t>2025-05-07 12:00:45</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-05-14 14:49:28</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>3859</v>
+        <v>2262</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1948,66 +1961,71 @@
         </is>
       </c>
       <c r="L21" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M21" t="n">
         <v>70</v>
       </c>
-      <c r="O21" t="n">
-        <v>0</v>
+      <c r="N21" t="n">
+        <v>39749</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-05-02 00:00:00</t>
         </is>
       </c>
       <c r="R21" s="1" t="n">
-        <v>0</v>
+        <v>-0.5925130208333333</v>
       </c>
       <c r="S21" s="1" t="n">
-        <v>0</v>
+        <v>-0.5250651041666666</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>251284</v>
+        <v>251548</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>40.5</v>
+        <v>19</v>
       </c>
       <c r="D22" t="n">
-        <v>297.0909090909091</v>
+        <v>206.90625</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-05-09 07:00:00</t>
+          <t>2025-05-07 12:36:05</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-05-09 07:40:30</t>
+          <t>2025-05-07 12:55:05</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>16340</v>
+        <v>13242</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2016,17 +2034,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L22" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M22" t="n">
         <v>70</v>
       </c>
       <c r="N22" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2034,57 +2052,57 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>39747</v>
+        <v>39749</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R22" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-1.416059027777778</v>
       </c>
       <c r="S22" s="1" t="n">
-        <v>-1.526104797974537</v>
+        <v>-1.348611111111111</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>251373</v>
+        <v>250923</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>34.5</v>
+        <v>32</v>
       </c>
       <c r="D23" t="n">
-        <v>310.8</v>
+        <v>109.46875</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2025-05-09 12:37:35</t>
+          <t>2025-05-08 08:22:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-05-09 13:12:05</t>
+          <t>2025-05-08 08:54:00</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-05-09 13:12:05</t>
+          <t>2025-05-08 08:54:00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-05-12 10:22:53</t>
+          <t>2025-05-08 10:43:28</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>17094</v>
+        <v>7006</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2093,70 +2111,75 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L23" t="n">
         <v>5</v>
       </c>
       <c r="M23" t="n">
-        <v>70</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="N23" t="n">
+        <v>39749</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>39749</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-04-07 00:00:00</t>
         </is>
       </c>
       <c r="R23" s="1" t="n">
-        <v>0</v>
+        <v>-1.514301215277778</v>
       </c>
       <c r="S23" s="1" t="n">
-        <v>0</v>
+        <v>-1.446853298611111</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>251463</v>
+        <v>251225</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>32.5</v>
+        <v>17</v>
       </c>
       <c r="D24" t="n">
-        <v>126.6727272727273</v>
+        <v>0</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-05-12 10:22:53</t>
+          <t>2025-05-08 10:43:28</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-05-12 10:55:23</t>
+          <t>2025-05-08 11:00:28</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-05-12 10:55:23</t>
+          <t>2025-05-08 11:00:28</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-05-12 13:02:03</t>
+          <t>2025-05-08 11:00:28</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>6967</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2165,70 +2188,75 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L24" t="n">
         <v>4</v>
       </c>
       <c r="M24" t="n">
-        <v>70</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="N24" t="n">
+        <v>39747</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>39747</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R24" s="1" t="n">
-        <v>0</v>
+        <v>-0.5261067708333333</v>
       </c>
       <c r="S24" s="1" t="n">
-        <v>0</v>
+        <v>-0.4586588541666667</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>251846</v>
+        <v>251227</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>34.5</v>
+        <v>15</v>
       </c>
       <c r="D25" t="n">
-        <v>207.1272727272727</v>
+        <v>0</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2025-05-12 13:02:03</t>
+          <t>2025-05-08 11:00:28</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-05-12 13:36:33</t>
+          <t>2025-05-08 11:15:28</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-05-12 13:36:33</t>
+          <t>2025-05-08 11:15:28</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-05-13 09:03:41</t>
+          <t>2025-05-08 11:15:28</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>11392</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2237,70 +2265,75 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M25" t="n">
-        <v>70</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="N25" t="n">
+        <v>39746</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>39746</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2025-05-30 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R25" s="1" t="n">
-        <v>0</v>
+        <v>-2.5365234375</v>
       </c>
       <c r="S25" s="1" t="n">
-        <v>0</v>
+        <v>-2.469075520833333</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251462</v>
+        <v>251421</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>30.5</v>
+        <v>17</v>
       </c>
       <c r="D26" t="n">
-        <v>113.2</v>
+        <v>81.9375</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-05-13 09:03:41</t>
+          <t>2025-05-08 11:15:28</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-05-13 09:34:11</t>
+          <t>2025-05-08 11:32:28</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-05-13 09:34:11</t>
+          <t>2025-05-08 11:32:28</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:23</t>
+          <t>2025-05-08 12:54:24</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>6226</v>
+        <v>5244</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2309,24 +2342,31 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M26" t="n">
-        <v>70</v>
-      </c>
-      <c r="O26" t="n">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>39762 (non in estrazione)</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P26" t="n">
-        <v>0</v>
+        <v>39762</v>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-08 00:00:00</t>
         </is>
       </c>
       <c r="R26" s="1" t="n">
@@ -2338,41 +2378,41 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>251520</v>
+        <v>251782</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>40.5</v>
+        <v>15</v>
       </c>
       <c r="D27" t="n">
-        <v>297.0909090909091</v>
+        <v>188.640625</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2025-05-13 11:27:23</t>
+          <t>2025-05-08 12:54:24</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-13 12:07:53</t>
+          <t>2025-05-08 13:09:24</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-05-13 12:07:53</t>
+          <t>2025-05-08 13:09:24</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-05-14 09:04:58</t>
+          <t>2025-05-09 08:18:02</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>16340</v>
+        <v>12073</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2381,66 +2421,71 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>CASON ;R6</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L27" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M27" t="n">
-        <v>70</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
+        <v>76</v>
+      </c>
+      <c r="N27" t="n">
+        <v>39754</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>39754</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2025-05-12 00:00:00</t>
+          <t>2025-05-16 00:00:00</t>
         </is>
       </c>
       <c r="R27" s="1" t="n">
-        <v>0</v>
+        <v>-0.4133138020833333</v>
       </c>
       <c r="S27" s="1" t="n">
-        <v>0</v>
+        <v>-0.3458658854166667</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>251259</v>
+        <v>251453</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>CASON</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>34.5</v>
+        <v>30</v>
       </c>
       <c r="D28" t="n">
-        <v>90.90909090909091</v>
+        <v>78.125</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2025-05-14 09:04:58</t>
+          <t>2025-05-09 08:18:02</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-05-14 09:39:28</t>
+          <t>2025-05-09 08:48:02</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-05-14 09:39:28</t>
+          <t>2025-05-09 08:48:02</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-05-14 11:10:23</t>
+          <t>2025-05-09 10:06:10</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2457,20 +2502,27 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="M28" t="n">
         <v>70</v>
       </c>
-      <c r="O28" t="n">
-        <v>0</v>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>39742 (non in estrazione)</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>39742</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R28" s="1" t="n">
@@ -2482,83 +2534,79 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>251706</v>
+        <v>251561</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D29" t="n">
-        <v>50.79365079365079</v>
+        <v>84.921875</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 10:06:10</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 10:25:10</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-05-12 07:00:00</t>
+          <t>2025-05-09 10:25:10</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-05-12 07:50:47</t>
+          <t>2025-05-09 11:50:05</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>3200</v>
+        <v>5435</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>foglio</t>
+          <t>bobina</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>39764 (esterno)</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>39764</v>
+        <v>0</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>2025-05-14 00:00:00</t>
+          <t>2025-05-07 00:00:00</t>
         </is>
       </c>
       <c r="R29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>251455</v>
+        <v>251546</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -2566,33 +2614,33 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D30" t="n">
-        <v>82.765625</v>
+        <v>101.03125</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2025-05-07 07:00:00</t>
+          <t>2025-05-09 11:50:05</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-09 12:05:05</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-05-07 07:19:00</t>
+          <t>2025-05-09 12:05:05</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-09 13:46:07</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>5297</v>
+        <v>6466</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2605,37 +2653,32 @@
         </is>
       </c>
       <c r="L30" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M30" t="n">
         <v>70</v>
       </c>
-      <c r="N30" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O30" t="n">
+        <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>2025-04-15 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R30" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>0</v>
       </c>
       <c r="S30" s="1" t="n">
-        <v>-0.3623372395833334</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>251391</v>
+        <v>251519</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2643,33 +2686,33 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D31" t="n">
-        <v>91.640625</v>
+        <v>205.859375</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2025-05-07 08:41:45</t>
+          <t>2025-05-09 13:46:07</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-09 14:07:07</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025-05-07 08:58:45</t>
+          <t>2025-05-09 14:07:07</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-12 09:32:59</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>5865</v>
+        <v>13175</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2682,37 +2725,32 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M31" t="n">
         <v>70</v>
       </c>
-      <c r="N31" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O31" t="n">
+        <v>0</v>
       </c>
       <c r="P31" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-06-10 00:00:00</t>
         </is>
       </c>
       <c r="R31" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>0</v>
       </c>
       <c r="S31" s="1" t="n">
-        <v>-0.4377821180555556</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>251395</v>
+        <v>251397</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2723,30 +2761,30 @@
         <v>17</v>
       </c>
       <c r="D32" t="n">
-        <v>35.34375</v>
+        <v>84.921875</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2025-05-07 10:30:24</t>
+          <t>2025-05-12 09:32:59</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-12 09:49:59</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025-05-07 10:47:24</t>
+          <t>2025-05-12 09:49:59</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-12 11:14:54</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>2262</v>
+        <v>5435</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2759,37 +2797,32 @@
         </is>
       </c>
       <c r="L32" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M32" t="n">
         <v>70</v>
       </c>
-      <c r="N32" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O32" t="n">
+        <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R32" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>0</v>
       </c>
       <c r="S32" s="1" t="n">
-        <v>-0.4741319444444445</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>251371</v>
+        <v>251594</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2797,33 +2830,33 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>101.03125</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2025-05-07 11:22:45</t>
+          <t>2025-05-12 11:14:54</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-12 11:31:54</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-12 11:31:54</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-12 13:12:56</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>6466</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -2841,34 +2874,27 @@
       <c r="M33" t="n">
         <v>70</v>
       </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>39666 (esterno)</t>
-        </is>
-      </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O33" t="n">
+        <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>39666</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>2025-04-24 00:00:00</t>
+          <t>2025-05-07 00:00:00</t>
         </is>
       </c>
       <c r="R33" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>0</v>
       </c>
       <c r="S33" s="1" t="n">
-        <v>-13.48732638888889</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>251396</v>
+        <v>250819</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -2879,30 +2905,30 @@
         <v>19</v>
       </c>
       <c r="D34" t="n">
-        <v>35.34375</v>
+        <v>133.234375</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2025-05-07 11:41:45</t>
+          <t>2025-05-12 13:12:56</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-05-07 12:00:45</t>
+          <t>2025-05-12 13:31:56</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025-05-07 12:00:45</t>
+          <t>2025-05-12 13:31:56</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-05-07 12:36:05</t>
+          <t>2025-05-13 07:45:10</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>2262</v>
+        <v>8527</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2920,32 +2946,27 @@
       <c r="M34" t="n">
         <v>70</v>
       </c>
-      <c r="N34" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O34" t="n">
+        <v>0</v>
       </c>
       <c r="P34" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>2025-05-02 00:00:00</t>
+          <t>2025-04-18 00:00:00</t>
         </is>
       </c>
       <c r="R34" s="1" t="n">
-        <v>-0.5925130208333333</v>
+        <v>0</v>
       </c>
       <c r="S34" s="1" t="n">
-        <v>-0.5250651041666666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>251548</v>
+        <v>251245</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -2953,33 +2974,33 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D35" t="n">
-        <v>206.90625</v>
+        <v>11.78125</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025-05-07 12:36:05</t>
+          <t>2025-05-13 07:45:10</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-05-07 12:55:05</t>
+          <t>2025-05-13 08:00:10</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025-05-07 12:55:05</t>
+          <t>2025-05-13 08:00:10</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-05-08 08:22:00</t>
+          <t>2025-05-13 08:11:57</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>13242</v>
+        <v>754</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -2988,41 +3009,36 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L35" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M35" t="n">
         <v>70</v>
       </c>
-      <c r="N35" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O35" t="n">
+        <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-03-28 00:00:00</t>
         </is>
       </c>
       <c r="R35" s="1" t="n">
-        <v>-1.416059027777778</v>
+        <v>0</v>
       </c>
       <c r="S35" s="1" t="n">
-        <v>-1.348611111111111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>250923</v>
+        <v>251247</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -3030,33 +3046,33 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D36" t="n">
-        <v>109.46875</v>
+        <v>420.84375</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2025-05-08 08:22:00</t>
+          <t>2025-05-13 08:11:57</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-05-08 08:54:00</t>
+          <t>2025-05-13 08:26:57</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025-05-08 08:54:00</t>
+          <t>2025-05-13 08:26:57</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:28</t>
+          <t>2025-05-14 07:27:47</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>7006</v>
+        <v>26934</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3065,41 +3081,36 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L36" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M36" t="n">
-        <v>76</v>
-      </c>
-      <c r="N36" t="n">
-        <v>39749</v>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0</v>
       </c>
       <c r="P36" t="n">
-        <v>39749</v>
+        <v>0</v>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>2025-04-07 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R36" s="1" t="n">
-        <v>-1.514301215277778</v>
+        <v>0</v>
       </c>
       <c r="S36" s="1" t="n">
-        <v>-1.446853298611111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>251225</v>
+        <v>251062</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -3107,33 +3118,33 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>353.5</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2025-05-08 10:43:28</t>
+          <t>2025-05-14 07:27:47</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-05-08 11:00:28</t>
+          <t>2025-05-14 07:42:47</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025-05-08 11:00:28</t>
+          <t>2025-05-14 07:42:47</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-05-08 11:00:28</t>
+          <t>2025-05-14 13:36:17</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>22624</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3142,75 +3153,70 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L37" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M37" t="n">
-        <v>76</v>
-      </c>
-      <c r="N37" t="n">
-        <v>39747</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>39747</v>
+        <v>0</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-23 00:00:00</t>
         </is>
       </c>
       <c r="R37" s="1" t="n">
-        <v>-0.5261067708333333</v>
+        <v>0</v>
       </c>
       <c r="S37" s="1" t="n">
-        <v>-0.4586588541666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>251227</v>
+        <v>251547</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>184.9154929577465</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2025-05-08 11:00:28</t>
+          <t>2025-05-08 07:00:00</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-05-08 11:15:28</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025-05-08 11:15:28</t>
+          <t>2025-05-08 07:34:00</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-05-08 11:15:28</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>13129</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3219,17 +3225,17 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L38" t="n">
         <v>4</v>
       </c>
       <c r="M38" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N38" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3237,57 +3243,57 @@
         </is>
       </c>
       <c r="P38" t="n">
-        <v>39746</v>
+        <v>39749</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>2025-05-05 00:00:00</t>
+          <t>2025-05-06 00:00:00</t>
         </is>
       </c>
       <c r="R38" s="1" t="n">
-        <v>-2.5365234375</v>
+        <v>-1.443691314548611</v>
       </c>
       <c r="S38" s="1" t="n">
-        <v>-2.469075520833333</v>
+        <v>-1.443691314548611</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>251421</v>
+        <v>250759</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D39" t="n">
-        <v>81.9375</v>
+        <v>118.2816901408451</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2025-05-08 11:15:28</t>
+          <t>2025-05-08 10:38:54</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-05-08 11:32:28</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025-05-08 11:32:28</t>
+          <t>2025-05-08 11:08:54</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-05-08 12:54:24</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>5244</v>
+        <v>8398</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3296,19 +3302,17 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M39" t="n">
         <v>76</v>
       </c>
-      <c r="N39" t="inlineStr">
-        <is>
-          <t>39762 (non in estrazione)</t>
-        </is>
+      <c r="N39" t="n">
+        <v>39747</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3316,57 +3320,57 @@
         </is>
       </c>
       <c r="P39" t="n">
-        <v>39762</v>
+        <v>39747</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>2025-05-08 00:00:00</t>
+          <t>2025-03-13 00:00:00</t>
         </is>
       </c>
       <c r="R39" s="1" t="n">
-        <v>0</v>
+        <v>-0.5466647104861111</v>
       </c>
       <c r="S39" s="1" t="n">
-        <v>0</v>
+        <v>-0.5466647104861111</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>251782</v>
+        <v>251564</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D40" t="n">
-        <v>188.640625</v>
+        <v>38.26760563380282</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2025-05-08 12:54:24</t>
+          <t>2025-05-08 13:07:11</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:24</t>
+          <t>2025-05-08 13:39:11</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025-05-08 13:09:24</t>
+          <t>2025-05-08 13:39:11</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-05-09 08:18:02</t>
+          <t>2025-05-08 14:17:27</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>12073</v>
+        <v>2717</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3375,75 +3379,70 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L40" t="n">
         <v>3</v>
       </c>
       <c r="M40" t="n">
-        <v>76</v>
-      </c>
-      <c r="N40" t="n">
-        <v>39754</v>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+        <v>70</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0</v>
       </c>
       <c r="P40" t="n">
-        <v>39754</v>
+        <v>0</v>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>2025-05-16 00:00:00</t>
+          <t>2025-05-07 00:00:00</t>
         </is>
       </c>
       <c r="R40" s="1" t="n">
-        <v>-0.4133138020833333</v>
+        <v>0</v>
       </c>
       <c r="S40" s="1" t="n">
-        <v>-0.3458658854166667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>251453</v>
+        <v>251626</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D41" t="n">
-        <v>78.125</v>
+        <v>176.056338028169</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2025-05-09 08:18:02</t>
+          <t>2025-05-08 14:17:27</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-05-09 08:48:02</t>
+          <t>2025-05-08 14:32:27</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025-05-09 08:48:02</t>
+          <t>2025-05-08 14:32:27</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-05-09 10:06:10</t>
+          <t>2025-05-09 09:28:31</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>5000</v>
+        <v>12500</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3461,22 +3460,15 @@
       <c r="M41" t="n">
         <v>70</v>
       </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>39742 (non in estrazione)</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O41" t="n">
+        <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>39742</v>
+        <v>0</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-04-30 00:00:00</t>
         </is>
       </c>
       <c r="R41" s="1" t="n">
@@ -3488,41 +3480,41 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>251561</v>
+        <v>251252</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D42" t="n">
-        <v>84.921875</v>
+        <v>212.4366197183099</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2025-05-09 10:06:10</t>
+          <t>2025-05-09 09:28:31</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-05-09 10:25:10</t>
+          <t>2025-05-09 09:49:31</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025-05-09 10:25:10</t>
+          <t>2025-05-09 09:49:31</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-05-09 11:50:05</t>
+          <t>2025-05-09 13:21:57</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>5435</v>
+        <v>15083</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3531,11 +3523,11 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L42" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M42" t="n">
         <v>70</v>
@@ -3548,7 +3540,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>2025-05-07 00:00:00</t>
+          <t>2025-05-23 00:00:00</t>
         </is>
       </c>
       <c r="R42" s="1" t="n">
@@ -3560,41 +3552,41 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>251546</v>
+        <v>251229</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C43" t="n">
         <v>15</v>
       </c>
       <c r="D43" t="n">
-        <v>101.03125</v>
+        <v>263.9295774647887</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2025-05-09 11:50:05</t>
+          <t>2025-05-09 13:21:57</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-05-09 12:05:05</t>
+          <t>2025-05-09 13:36:57</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025-05-09 12:05:05</t>
+          <t>2025-05-09 13:36:57</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-05-09 13:46:07</t>
+          <t>2025-05-12 10:00:53</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>6466</v>
+        <v>18739</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3603,24 +3595,31 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L43" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M43" t="n">
         <v>70</v>
       </c>
-      <c r="O43" t="n">
-        <v>0</v>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>39723 (esterno)</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P43" t="n">
-        <v>0</v>
+        <v>39723</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R43" s="1" t="n">
@@ -3632,41 +3631,41 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>251519</v>
+        <v>245350</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D44" t="n">
-        <v>205.859375</v>
+        <v>393.943661971831</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2025-05-09 13:46:07</t>
+          <t>2025-05-12 10:00:53</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:07</t>
+          <t>2025-05-12 10:23:53</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025-05-09 14:07:07</t>
+          <t>2025-05-12 10:23:53</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-05-12 09:32:59</t>
+          <t>2025-05-13 08:57:49</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>13175</v>
+        <v>27970</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3675,11 +3674,11 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
         </is>
       </c>
       <c r="L44" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M44" t="n">
         <v>70</v>
@@ -3692,7 +3691,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>2025-06-10 00:00:00</t>
+          <t>2025-12-31 00:00:00</t>
         </is>
       </c>
       <c r="R44" s="1" t="n">
@@ -3704,41 +3703,41 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>251397</v>
+        <v>251485</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D45" t="n">
-        <v>84.921875</v>
+        <v>67.71830985915493</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2025-05-12 09:32:59</t>
+          <t>2025-05-13 08:57:49</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-05-12 09:49:59</t>
+          <t>2025-05-13 09:22:49</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025-05-12 09:49:59</t>
+          <t>2025-05-13 09:22:49</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-05-12 11:14:54</t>
+          <t>2025-05-13 10:30:32</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>5435</v>
+        <v>4808</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3751,7 +3750,7 @@
         </is>
       </c>
       <c r="L45" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M45" t="n">
         <v>70</v>
@@ -3764,7 +3763,7 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>2025-04-28 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R45" s="1" t="n">
@@ -3776,41 +3775,41 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>251594</v>
+        <v>251761</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C46" t="n">
         <v>17</v>
       </c>
       <c r="D46" t="n">
-        <v>101.03125</v>
+        <v>187.0281690140845</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2025-05-12 11:14:54</t>
+          <t>2025-05-13 10:30:32</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-05-12 11:31:54</t>
+          <t>2025-05-13 10:47:32</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025-05-12 11:31:54</t>
+          <t>2025-05-13 10:47:32</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-05-12 13:12:56</t>
+          <t>2025-05-13 13:54:34</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>6466</v>
+        <v>13279</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3836,7 +3835,7 @@
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>2025-05-07 00:00:00</t>
+          <t>2025-05-19 00:00:00</t>
         </is>
       </c>
       <c r="R46" s="1" t="n">
@@ -3848,41 +3847,41 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>250819</v>
+        <v>251464</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D47" t="n">
-        <v>133.234375</v>
+        <v>100.7464788732394</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2025-05-12 13:12:56</t>
+          <t>2025-05-13 13:54:34</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-05-12 13:31:56</t>
+          <t>2025-05-13 14:09:34</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025-05-12 13:31:56</t>
+          <t>2025-05-13 14:09:34</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-05-13 07:45:10</t>
+          <t>2025-05-14 07:50:19</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>8527</v>
+        <v>7153</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3895,7 +3894,7 @@
         </is>
       </c>
       <c r="L47" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M47" t="n">
         <v>70</v>
@@ -3908,7 +3907,7 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>2025-04-18 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R47" s="1" t="n">
@@ -3920,41 +3919,41 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>251245</v>
+        <v>251467</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D48" t="n">
-        <v>11.78125</v>
+        <v>87.69014084507042</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2025-05-13 07:45:10</t>
+          <t>2025-05-14 07:50:19</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-05-13 08:00:10</t>
+          <t>2025-05-14 08:09:19</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025-05-13 08:00:10</t>
+          <t>2025-05-14 08:09:19</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-05-13 08:11:57</t>
+          <t>2025-05-14 09:37:00</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>754</v>
+        <v>6226</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -3963,11 +3962,11 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L48" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M48" t="n">
         <v>70</v>
@@ -3980,7 +3979,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>2025-03-28 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R48" s="1" t="n">
@@ -3992,41 +3991,41 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>251247</v>
+        <v>251557</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C49" t="n">
         <v>15</v>
       </c>
       <c r="D49" t="n">
-        <v>420.84375</v>
+        <v>94.43661971830986</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2025-05-13 08:11:57</t>
+          <t>2025-05-14 09:37:00</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-05-13 08:26:57</t>
+          <t>2025-05-14 09:52:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025-05-13 08:26:57</t>
+          <t>2025-05-14 09:52:00</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-05-14 07:27:47</t>
+          <t>2025-05-14 11:26:27</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>26934</v>
+        <v>6705</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4035,11 +4034,11 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L49" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M49" t="n">
         <v>70</v>
@@ -4052,7 +4051,7 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R49" s="1" t="n">
@@ -4064,41 +4063,41 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>251062</v>
+        <v>245089</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>BIMEC 2</t>
+          <t>BIMEC 5</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D50" t="n">
-        <v>353.5</v>
+        <v>1727.676056338028</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2025-05-14 07:27:47</t>
+          <t>2025-05-14 11:26:27</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-05-14 07:42:47</t>
+          <t>2025-05-14 12:00:27</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025-05-14 07:42:47</t>
+          <t>2025-05-14 12:00:27</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-05-14 13:36:17</t>
+          <t>2025-05-20 08:48:07</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>22624</v>
+        <v>122665</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4107,14 +4106,14 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
         </is>
       </c>
       <c r="L50" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M50" t="n">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="O50" t="n">
         <v>0</v>
@@ -4124,7 +4123,7 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>2025-05-23 00:00:00</t>
+          <t>2025-12-31 00:00:00</t>
         </is>
       </c>
       <c r="R50" s="1" t="n">
@@ -4136,18 +4135,18 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>251547</v>
+        <v>251742</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D51" t="n">
-        <v>184.9154929577465</v>
+        <v>134.8524590163935</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -4156,21 +4155,21 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025-05-08 07:34:00</t>
+          <t>2025-05-08 07:30:00</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>13129</v>
+        <v>8226</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -4201,53 +4200,53 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>2025-05-06 00:00:00</t>
+          <t>2025-05-15 00:00:00</t>
         </is>
       </c>
       <c r="R51" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-1.406147540983796</v>
       </c>
       <c r="S51" s="1" t="n">
-        <v>-1.443691314548611</v>
+        <v>-1.406147540983796</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>250759</v>
+        <v>251840</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D52" t="n">
-        <v>118.2816901408451</v>
+        <v>93.67213114754098</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2025-05-08 10:38:54</t>
+          <t>2025-05-08 09:44:51</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025-05-08 11:08:54</t>
+          <t>2025-05-08 10:09:51</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>8398</v>
+        <v>5714</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -4256,17 +4255,17 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L52" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M52" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N52" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4274,57 +4273,57 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>39747</v>
+        <v>39758</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>2025-03-13 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R52" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.4885587431712963</v>
       </c>
       <c r="S52" s="1" t="n">
-        <v>-0.5466647104861111</v>
+        <v>-0.4885587431712963</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>251564</v>
+        <v>251456</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D53" t="n">
-        <v>38.26760563380282</v>
+        <v>147.5245901639344</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2025-05-08 13:07:11</t>
+          <t>2025-05-08 11:43:31</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-05-08 13:39:11</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025-05-08 13:39:11</t>
+          <t>2025-05-08 12:13:31</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>2025-05-08 14:17:27</t>
+          <t>2025-05-08 14:41:02</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>2717</v>
+        <v>8999</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4342,61 +4341,66 @@
       <c r="M53" t="n">
         <v>70</v>
       </c>
-      <c r="O53" t="n">
-        <v>0</v>
+      <c r="N53" t="n">
+        <v>39746</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="P53" t="n">
-        <v>0</v>
+        <v>39746</v>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>2025-05-07 00:00:00</t>
+          <t>2025-05-09 00:00:00</t>
         </is>
       </c>
       <c r="R53" s="1" t="n">
-        <v>0</v>
+        <v>-2.611839708564815</v>
       </c>
       <c r="S53" s="1" t="n">
-        <v>0</v>
+        <v>-2.611839708564815</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>251626</v>
+        <v>251416</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D54" t="n">
-        <v>176.056338028169</v>
+        <v>183.9672131147541</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2025-05-08 14:17:27</t>
+          <t>2025-05-08 14:41:02</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-05-08 14:32:27</t>
+          <t>2025-05-09 07:06:02</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025-05-08 14:32:27</t>
+          <t>2025-05-09 07:06:02</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>2025-05-09 09:28:31</t>
+          <t>2025-05-09 10:10:00</t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>12500</v>
+        <v>11222</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -4409,11 +4413,14 @@
         </is>
       </c>
       <c r="L54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M54" t="n">
         <v>70</v>
       </c>
+      <c r="N54" t="n">
+        <v>39755</v>
+      </c>
       <c r="O54" t="n">
         <v>0</v>
       </c>
@@ -4422,7 +4429,7 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>2025-04-30 00:00:00</t>
+          <t>2025-04-23 00:00:00</t>
         </is>
       </c>
       <c r="R54" s="1" t="n">
@@ -4434,41 +4441,41 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>251252</v>
+        <v>251566</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D55" t="n">
-        <v>212.4366197183099</v>
+        <v>112.9344262295082</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2025-05-09 09:28:31</t>
+          <t>2025-05-09 10:10:00</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-05-09 09:49:31</t>
+          <t>2025-05-09 10:40:00</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025-05-09 09:49:31</t>
+          <t>2025-05-09 10:40:00</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>2025-05-09 13:21:57</t>
+          <t>2025-05-09 12:32:57</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>15083</v>
+        <v>6889</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -4477,11 +4484,11 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L55" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M55" t="n">
         <v>70</v>
@@ -4494,7 +4501,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>2025-05-23 00:00:00</t>
+          <t>2025-05-07 00:00:00</t>
         </is>
       </c>
       <c r="R55" s="1" t="n">
@@ -4506,41 +4513,41 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>251229</v>
+        <v>251424</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D56" t="n">
-        <v>263.9295774647887</v>
+        <v>158.3934426229508</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2025-05-09 13:21:57</t>
+          <t>2025-05-09 12:32:57</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-05-09 13:36:57</t>
+          <t>2025-05-09 12:52:57</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025-05-09 13:36:57</t>
+          <t>2025-05-09 12:52:57</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>2025-05-12 10:00:53</t>
+          <t>2025-05-12 07:31:20</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>18739</v>
+        <v>9662</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -4549,31 +4556,24 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L56" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M56" t="n">
         <v>70</v>
       </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>39723 (esterno)</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
+      <c r="O56" t="n">
+        <v>0</v>
       </c>
       <c r="P56" t="n">
-        <v>39723</v>
+        <v>0</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R56" s="1" t="n">
@@ -4585,41 +4585,41 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>245350</v>
+        <v>244355</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D57" t="n">
-        <v>393.943661971831</v>
+        <v>70.65573770491804</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2025-05-12 10:00:53</t>
+          <t>2025-05-12 07:31:20</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-05-12 10:23:53</t>
+          <t>2025-05-12 07:51:20</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025-05-12 10:23:53</t>
+          <t>2025-05-12 07:51:20</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>2025-05-13 08:57:49</t>
+          <t>2025-05-12 09:02:00</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>27970</v>
+        <v>4310</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -4628,11 +4628,11 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L57" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="M57" t="n">
         <v>70</v>
@@ -4645,7 +4645,7 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>2025-12-31 00:00:00</t>
+          <t>2025-05-08 00:00:00</t>
         </is>
       </c>
       <c r="R57" s="1" t="n">
@@ -4657,41 +4657,41 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>251485</v>
+        <v>251505</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C58" t="n">
         <v>25</v>
       </c>
       <c r="D58" t="n">
-        <v>67.71830985915493</v>
+        <v>233.6885245901639</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2025-05-13 08:57:49</t>
+          <t>2025-05-12 09:02:00</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-05-13 09:22:49</t>
+          <t>2025-05-12 09:27:00</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>2025-05-13 09:22:49</t>
+          <t>2025-05-12 09:27:00</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>2025-05-13 10:30:32</t>
+          <t>2025-05-12 13:20:41</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>4808</v>
+        <v>14255</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -4717,7 +4717,7 @@
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>2025-04-23 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R58" s="1" t="n">
@@ -4729,41 +4729,41 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>251761</v>
+        <v>244023</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D59" t="n">
-        <v>187.0281690140845</v>
+        <v>16.34426229508197</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2025-05-13 10:30:32</t>
+          <t>2025-05-12 13:20:41</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-05-13 10:47:32</t>
+          <t>2025-05-12 13:45:41</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>2025-05-13 10:47:32</t>
+          <t>2025-05-12 13:45:41</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>2025-05-13 13:54:34</t>
+          <t>2025-05-12 14:02:01</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>13279</v>
+        <v>997</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -4776,7 +4776,7 @@
         </is>
       </c>
       <c r="L59" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M59" t="n">
         <v>70</v>
@@ -4789,7 +4789,7 @@
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>2025-05-19 00:00:00</t>
+          <t>2024-09-30 00:00:00</t>
         </is>
       </c>
       <c r="R59" s="1" t="n">
@@ -4801,41 +4801,41 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>251464</v>
+        <v>251061</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D60" t="n">
-        <v>100.7464788732394</v>
+        <v>393.3934426229508</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2025-05-13 13:54:34</t>
+          <t>2025-05-12 14:02:01</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-05-13 14:09:34</t>
+          <t>2025-05-12 14:22:01</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>2025-05-13 14:09:34</t>
+          <t>2025-05-12 14:22:01</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>2025-05-14 07:50:19</t>
+          <t>2025-05-13 12:55:25</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>7153</v>
+        <v>23997</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4844,11 +4844,11 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R9</t>
         </is>
       </c>
       <c r="L60" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M60" t="n">
         <v>70</v>
@@ -4861,7 +4861,7 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-05 00:00:00</t>
         </is>
       </c>
       <c r="R60" s="1" t="n">
@@ -4873,41 +4873,41 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>251467</v>
+        <v>251260</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D61" t="n">
-        <v>87.69014084507042</v>
+        <v>153.5901639344262</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2025-05-14 07:50:19</t>
+          <t>2025-05-13 12:55:25</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-05-14 08:09:19</t>
+          <t>2025-05-13 13:15:25</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>2025-05-14 08:09:19</t>
+          <t>2025-05-13 13:15:25</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>2025-05-14 09:37:00</t>
+          <t>2025-05-14 07:49:00</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>6226</v>
+        <v>9369</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -4916,11 +4916,11 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L61" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M61" t="n">
         <v>70</v>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>2025-05-09 00:00:00</t>
+          <t>2025-05-22 00:00:00</t>
         </is>
       </c>
       <c r="R61" s="1" t="n">
@@ -4945,41 +4945,41 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>251557</v>
+        <v>251795</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D62" t="n">
-        <v>94.43661971830986</v>
+        <v>307.1967213114754</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2025-05-14 09:37:00</t>
+          <t>2025-05-14 07:49:00</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-05-14 09:52:00</t>
+          <t>2025-05-14 08:09:00</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>2025-05-14 09:52:00</t>
+          <t>2025-05-14 08:09:00</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>2025-05-14 11:26:27</t>
+          <t>2025-05-14 13:16:12</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>6705</v>
+        <v>18739</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -4988,11 +4988,11 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R9</t>
         </is>
       </c>
       <c r="L62" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M62" t="n">
         <v>70</v>
@@ -5005,7 +5005,7 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>2025-05-15 00:00:00</t>
+          <t>2025-06-19 00:00:00</t>
         </is>
       </c>
       <c r="R62" s="1" t="n">
@@ -5017,41 +5017,41 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>245089</v>
+        <v>251346</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>BIMEC 5</t>
+          <t>R10</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D63" t="n">
-        <v>1727.676056338028</v>
+        <v>63.26229508196721</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2025-05-14 11:26:27</t>
+          <t>2025-05-14 13:16:12</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-05-14 12:00:27</t>
+          <t>2025-05-14 13:46:12</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>2025-05-14 12:00:27</t>
+          <t>2025-05-14 13:46:12</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>2025-05-20 08:48:07</t>
+          <t>2025-05-14 14:49:28</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>122665</v>
+        <v>3859</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -5060,14 +5060,14 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;R12 ;R9</t>
+          <t>BIMEC 2 ;BIMEC 4 ;BIMEC 5 ;CASON ;R10 ;R3 ;R6 ;R9</t>
         </is>
       </c>
       <c r="L63" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M63" t="n">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="O63" t="n">
         <v>0</v>
@@ -5077,7 +5077,7 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>2025-12-31 00:00:00</t>
+          <t>2025-04-28 00:00:00</t>
         </is>
       </c>
       <c r="R63" s="1" t="n">

</xml_diff>